<commit_message>
creating notebooks + data cleaning first draft
</commit_message>
<xml_diff>
--- a/data/Germany_EC1B1_Dataset.xlsx
+++ b/data/Germany_EC1B1_Dataset.xlsx
@@ -6,8 +6,8 @@
     <x:workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="10365" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="International Financial Statis" sheetId="1" r:id="Reddd158b51724d61"/>
-    <x:sheet name="Tooltip" sheetId="2" r:id="R451eec878a8d430d"/>
+    <x:sheet name="International Financial Statis" sheetId="1" r:id="R8e2c1e69392c4d31"/>
+    <x:sheet name="Tooltip" sheetId="2" r:id="R44077f84d1d041df"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -138,7 +138,7 @@
       <x:c s="0"/>
       <x:c s="0"/>
     </x:row>
-    <x:row ht="16.5" customHeight="1">
+    <x:row ht="17.25" customHeight="1">
       <x:c s="0"/>
       <x:c s="0"/>
       <x:c s="5" t="str">
@@ -7374,9 +7374,249 @@
         <x:v>66.3678165624309</x:v>
       </x:c>
     </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Jan 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>78.3694166018768</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.6918</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>68950.3667233367</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>66.7174841249911</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Feb 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>78.5858181408675</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.676</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>69982.7949030696</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>66.9972272165096</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Mar 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>87.1296714950913</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.7045</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>69567.6986922397</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>66.9972272165096</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Apr 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>79.7800340412234</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.6882</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>69701.9849596987</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>67.137087460431</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>May 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>81.2708001987146</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.6617</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>70727.7233721584</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>67.2769590061902</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Jun 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>81.7597073793972</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.684</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>71640.0798160129</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>67.3468947790698</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Jul 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>78.7942048080437</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.6399</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>71072.396009484</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>67.3468947790698</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Aug 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>75.9649550575362</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.5707</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>72425.7385732047</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>67.5567020977087</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Sep 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>86.4964966217483</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.5697</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>73197.5736206214</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>67.7665094163475</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Oct 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>92.643903303446</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.5233</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>75011.9268302281</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>68.256048524667</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="16.5" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Nov 1990</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>89.4619991931018</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>1.487</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>76166.0747088573</x:v>
+      </x:c>
+      <x:c s="9">
+        <x:v>68.1161769789078</x:v>
+      </x:c>
+    </x:row>
+    <x:row ht="17.25" customHeight="1">
+      <x:c s="6" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="7" t="str">
+        <x:v>Dec 1990</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>83.8115145639013</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>1.492</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>77064.2076742664</x:v>
+      </x:c>
+      <x:c s="8">
+        <x:v>68.1861127517874</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:mergeCells count="2">
-    <x:mergeCell ref="A3:A363"/>
+    <x:mergeCell ref="A3:A375"/>
     <x:mergeCell ref="A1:F1"/>
   </x:mergeCells>
   <x:pageMargins left="1.18" right="0.79" top="0.79" bottom="0.79" header="0" footer="0"/>
@@ -16076,6 +16316,294 @@
 Time: Dec 1989</x:v>
       </x:c>
     </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Jan 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jan 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jan 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jan 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jan 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Feb 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Feb 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Feb 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Feb 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Feb 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Mar 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Mar 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Mar 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Mar 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Mar 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Apr 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Apr 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Apr 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Apr 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Apr 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>May 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: May 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: May 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: May 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: May 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Jun 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jun 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jun 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jun 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jun 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Jul 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jul 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jul 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jul 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Jul 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Aug 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Aug 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Aug 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Aug 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Aug 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Sep 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Sep 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Sep 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Sep 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Sep 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Oct 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Oct 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Oct 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Oct 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Oct 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Nov 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Nov 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Nov 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Nov 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Nov 1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row customHeight="0">
+      <x:c s="0" t="str">
+        <x:v>Germany</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Dec 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Dec 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Dec 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Dec 1990</x:v>
+      </x:c>
+      <x:c s="0" t="str">
+        <x:v>Country: Germany
+Time: Dec 1990</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:mergeCells count="1">
     <x:mergeCell ref="A1:A1"/>

</xml_diff>